<commit_message>
Burndown Chart Sprint 4 Completed
Made the chart that relates to the data in the table
</commit_message>
<xml_diff>
--- a/Project Management/BurnDown Charts/BurnDown Chart.xlsx
+++ b/Project Management/BurnDown Charts/BurnDown Chart.xlsx
@@ -1,13 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
+  <workbookPr autoCompressPictures="0"/>
+  <bookViews>
+    <workbookView xWindow="240" yWindow="0" windowWidth="25600" windowHeight="15620" tabRatio="500"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Table Sprint 4" sheetId="1" r:id="rId3"/>
-    <sheet state="visible" name="Sprint 4 Chart" sheetId="2" r:id="rId4"/>
+    <sheet name="Table Sprint 4" sheetId="1" r:id="rId1"/>
+    <sheet name="Sprint 4 Chart" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -116,32 +124,50 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="14.0"/>
-    </font>
-    <font>
-      <sz val="12.0"/>
-    </font>
-    <font>
-      <sz val="12.0"/>
-      <name val="Times New Roman"/>
-    </font>
-    <font/>
-    <font>
+      <sz val="14"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="12"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Inconsolata"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="9">
@@ -149,7 +175,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -195,7 +221,13 @@
     </fill>
   </fills>
   <borders count="20">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -209,6 +241,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -217,9 +250,11 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -228,9 +263,11 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -239,9 +276,11 @@
       <right style="thin">
         <color rgb="FF0000FF"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -256,6 +295,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -270,8 +310,10 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -281,8 +323,10 @@
       <bottom style="thin">
         <color rgb="FF0000FF"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF0000FF"/>
       </right>
@@ -292,6 +336,7 @@
       <bottom style="thin">
         <color rgb="FF0000FF"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -306,8 +351,10 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -317,8 +364,10 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -328,14 +377,18 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -344,11 +397,18 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -363,8 +423,10 @@
       <bottom style="thin">
         <color rgb="FFFF0000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -374,6 +436,7 @@
       <bottom style="thin">
         <color rgb="FFFF0000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -382,216 +445,1168 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  <cellStyleXfs count="11">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="57">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="7" fillId="6" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="9" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="10" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="11" fillId="6" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="3" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="12" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="12" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="12" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="12" fillId="6" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="12" fillId="6" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="13" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="14" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="14" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="14" fillId="6" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="15" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="16" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="16" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="16" fillId="6" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="17" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="14" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="7" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="7" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="7" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="7" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="7" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="7" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="8" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="8" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="18" fillId="8" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="19" fillId="8" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+  <cellStyles count="11">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Sprint 4 Burndown</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Stories Remaining</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Table Sprint 4'!$B$1:$P$1</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>Total Hours</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Day 1 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Day 2 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Day 3 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Day 4 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Day 5 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Day 6 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Day 7 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Day 8 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Day 9 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Day 10 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Day 11 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Day 12 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Day 13 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Day 14 (Hours)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Table Sprint 4'!$B$26:$P$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Stories Completed</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Table Sprint 4'!$B$1:$P$1</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>Total Hours</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Day 1 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Day 2 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Day 3 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Day 4 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Day 5 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Day 6 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Day 7 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Day 8 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Day 9 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Day 10 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Day 11 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Day 12 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Day 13 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Day 14 (Hours)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Table Sprint 4'!$B$27:$P$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>13.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="2047056680"/>
+        <c:axId val="-2114617528"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Remaining Effort</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Table Sprint 4'!$B$1:$P$1</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>Total Hours</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Day 1 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Day 2 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Day 3 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Day 4 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Day 5 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Day 6 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Day 7 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Day 8 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Day 9 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Day 10 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Day 11 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Day 12 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Day 13 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Day 14 (Hours)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Table Sprint 4'!$B$24:$P$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>76.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>71.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>65.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>53.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Ideal BurnDown</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Table Sprint 4'!$B$1:$P$1</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>Total Hours</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Day 1 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Day 2 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Day 3 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Day 4 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Day 5 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Day 6 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Day 7 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Day 8 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Day 9 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Day 10 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Day 11 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Day 12 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Day 13 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Day 14 (Hours)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Table Sprint 4'!$B$25:$P$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>76.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>70.57142857142857</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>65.14285714285714</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>59.71428571428571</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>54.28571428571428</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>48.85714285714285</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43.42857142857141</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>37.99999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>32.57142857142856</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>27.14285714285712</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>21.7142857142857</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>16.28571428571426</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10.85714285714283</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.428571428571406</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-2.30926389122033E-14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2047056680"/>
+        <c:axId val="-2114617528"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2047056680"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2114617528"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2114617528"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2047056680"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>914401</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1003301</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="100000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </a:style>
+    </a:spDef>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
+  <a:extraClrSchemeLst/>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="36.29"/>
+    <col min="1" max="1" width="36.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="33.0" customHeight="1">
+    <row r="1" spans="1:16" ht="33" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -641,668 +1656,668 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:16" ht="15">
       <c r="A2" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="5">
-        <f t="shared" ref="B2:B14" si="1">sum(C2:P2)</f>
+        <f t="shared" ref="B2:B14" si="0">SUM(C2:P2)</f>
         <v>3</v>
       </c>
       <c r="C2" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D2" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E2" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F2" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G2" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="H2" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I2" s="7">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="J2" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="K2" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="L2" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="M2" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="N2" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="O2" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="P2" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:16" ht="15">
       <c r="A3" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="C3" s="6">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D3" s="6">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E3" s="7">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="F3" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G3" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="H3" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I3" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="J3" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="K3" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="L3" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="M3" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="N3" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="O3" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="P3" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:16" ht="15">
       <c r="A4" s="8" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="C4" s="9">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D4" s="9">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E4" s="9">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F4" s="9">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G4" s="9">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="H4" s="9">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I4" s="9">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="J4" s="9">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="K4" s="9">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="L4" s="9">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="M4" s="9">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="N4" s="9">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="O4" s="10">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="P4" s="11">
-        <v>0.0</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:16" ht="15">
       <c r="A5" s="8" t="s">
         <v>19</v>
       </c>
       <c r="B5" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="C5" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="9">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="F5" s="9">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G5" s="9">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="H5" s="9">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="I5" s="9">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="J5" s="9">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="K5" s="9">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="L5" s="9">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="M5" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="N5" s="10">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="O5" s="9">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="P5" s="11">
-        <v>0.0</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:16" ht="15">
       <c r="A6" s="12" t="s">
         <v>20</v>
       </c>
       <c r="B6" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="C6" s="6">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="6">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E6" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F6" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G6" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="H6" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I6" s="6">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="J6" s="6">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="K6" s="6"/>
       <c r="L6" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="M6" s="6">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="N6" s="6">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="O6" s="7">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="P6" s="13">
-        <v>0.0</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:16" ht="15">
       <c r="A7" s="12" t="s">
         <v>21</v>
       </c>
       <c r="B7" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C7" s="14">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D7" s="14">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E7" s="14">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F7" s="14">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G7" s="14">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="H7" s="14">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I7" s="14">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="J7" s="14">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="K7" s="14">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="L7" s="14">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="M7" s="14">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="N7" s="15">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="O7" s="14">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="P7" s="16">
-        <v>0.0</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:16" ht="30">
       <c r="A8" s="17" t="s">
         <v>22</v>
       </c>
       <c r="B8" s="18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="C8" s="19">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="D8" s="19">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E8" s="20">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="F8" s="21">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G8" s="21">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="H8" s="21">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I8" s="21">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="J8" s="21">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="K8" s="21">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="L8" s="21">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="M8" s="21">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="N8" s="21">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="O8" s="21">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="P8" s="21">
-        <v>0.0</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:16" ht="15">
       <c r="A9" s="22" t="s">
         <v>23</v>
       </c>
       <c r="B9" s="23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="C9" s="24">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D9" s="24">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E9" s="24">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F9" s="25">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G9" s="25">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="H9" s="25">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="I9" s="25">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="J9" s="25">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="K9" s="25">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="L9" s="25">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="M9" s="25">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="N9" s="26">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="O9" s="25">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="P9" s="25">
-        <v>0.0</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:16" ht="15">
       <c r="A10" s="22" t="s">
         <v>24</v>
       </c>
       <c r="B10" s="23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="C10" s="24">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D10" s="24">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E10" s="24">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F10" s="24">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G10" s="24">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="H10" s="24">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I10" s="24">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="J10" s="24">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="K10" s="24">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="L10" s="24">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="M10" s="24">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="N10" s="27">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="O10" s="24">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="P10" s="24">
-        <v>0.0</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:16" ht="15">
       <c r="A11" s="22" t="s">
         <v>25</v>
       </c>
       <c r="B11" s="23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C11" s="24">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D11" s="24">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E11" s="24">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F11" s="24">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G11" s="24">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="H11" s="24">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I11" s="24">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="J11" s="24">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="K11" s="24">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="L11" s="27">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="M11" s="24">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="N11" s="24">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="O11" s="24">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="P11" s="24">
-        <v>0.0</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:16" ht="15">
       <c r="A12" s="28" t="s">
         <v>26</v>
       </c>
       <c r="B12" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C12" s="30">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D12" s="30">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E12" s="30">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F12" s="30">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G12" s="30">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="H12" s="30">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I12" s="30">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="J12" s="30">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="K12" s="30">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="L12" s="31">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="M12" s="30">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="N12" s="30">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="O12" s="30">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="P12" s="30">
-        <v>0.0</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:16" ht="15">
       <c r="A13" s="32" t="s">
         <v>27</v>
       </c>
       <c r="B13" s="33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C13" s="34">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D13" s="34">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E13" s="34">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F13" s="34">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G13" s="34">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="H13" s="34">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I13" s="34">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="J13" s="34">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="K13" s="34">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="L13" s="35">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="M13" s="34">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="N13" s="34">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="O13" s="34">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="P13" s="34">
-        <v>0.0</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:16" ht="15">
       <c r="A14" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B14" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C14" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D14" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E14" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F14" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G14" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="H14" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I14" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="J14" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="K14" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="L14" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="M14" s="7">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="N14" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="O14" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="P14" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:16" ht="15">
       <c r="A15" s="36"/>
       <c r="B15" s="29"/>
       <c r="C15" s="37"/>
@@ -1320,7 +2335,7 @@
       <c r="O15" s="37"/>
       <c r="P15" s="37"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:16" ht="15">
       <c r="A16" s="38"/>
       <c r="B16" s="39"/>
       <c r="C16" s="40"/>
@@ -1338,7 +2353,7 @@
       <c r="O16" s="40"/>
       <c r="P16" s="40"/>
     </row>
-    <row r="17">
+    <row r="17" spans="1:16" ht="15">
       <c r="A17" s="38"/>
       <c r="B17" s="39"/>
       <c r="C17" s="41"/>
@@ -1356,7 +2371,7 @@
       <c r="O17" s="40"/>
       <c r="P17" s="40"/>
     </row>
-    <row r="18">
+    <row r="18" spans="1:16" ht="15">
       <c r="A18" s="38"/>
       <c r="B18" s="42"/>
       <c r="C18" s="43"/>
@@ -1374,7 +2389,7 @@
       <c r="O18" s="40"/>
       <c r="P18" s="40"/>
     </row>
-    <row r="19">
+    <row r="19" spans="1:16" ht="15">
       <c r="A19" s="4"/>
       <c r="B19" s="5"/>
       <c r="C19" s="44"/>
@@ -1392,7 +2407,7 @@
       <c r="O19" s="44"/>
       <c r="P19" s="44"/>
     </row>
-    <row r="20">
+    <row r="20" spans="1:16" ht="15">
       <c r="A20" s="45"/>
       <c r="B20" s="46"/>
       <c r="C20" s="47"/>
@@ -1410,7 +2425,7 @@
       <c r="O20" s="47"/>
       <c r="P20" s="47"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:16" ht="15">
       <c r="A21" s="4"/>
       <c r="B21" s="5"/>
       <c r="C21" s="44"/>
@@ -1428,7 +2443,7 @@
       <c r="O21" s="44"/>
       <c r="P21" s="44"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:16" ht="15">
       <c r="A22" s="48"/>
       <c r="B22" s="5"/>
       <c r="C22" s="49"/>
@@ -1446,7 +2461,7 @@
       <c r="O22" s="49"/>
       <c r="P22" s="49"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:16" ht="15">
       <c r="A23" s="48"/>
       <c r="B23" s="5"/>
       <c r="C23" s="50"/>
@@ -1464,7 +2479,7 @@
       <c r="O23" s="50"/>
       <c r="P23" s="50"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:16" ht="15">
       <c r="A24" s="51" t="s">
         <v>29</v>
       </c>
@@ -1473,63 +2488,63 @@
         <v>76</v>
       </c>
       <c r="C24" s="52">
-        <f t="shared" ref="C24:P24" si="2">SUM(B24-SUM(C2:C23))</f>
+        <f t="shared" ref="C24:P24" si="1">SUM(B24-SUM(C2:C23))</f>
         <v>71</v>
       </c>
       <c r="D24" s="52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>65</v>
       </c>
       <c r="E24" s="52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>57</v>
       </c>
       <c r="F24" s="52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>57</v>
       </c>
       <c r="G24" s="52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>57</v>
       </c>
       <c r="H24" s="52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>53</v>
       </c>
       <c r="I24" s="52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>41</v>
       </c>
       <c r="J24" s="52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="K24" s="52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="L24" s="52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="M24" s="52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="N24" s="53">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="O24" s="52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P24" s="52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:16" ht="15">
       <c r="A25" s="51" t="s">
         <v>30</v>
       </c>
@@ -1538,63 +2553,63 @@
         <v>76</v>
       </c>
       <c r="C25" s="52">
-        <f t="shared" ref="C25:P25" si="3">B25-$B25/14</f>
-        <v>70.57142857</v>
+        <f t="shared" ref="C25:P25" si="2">B25-$B25/14</f>
+        <v>70.571428571428569</v>
       </c>
       <c r="D25" s="52">
-        <f t="shared" si="3"/>
-        <v>65.14285714</v>
+        <f t="shared" si="2"/>
+        <v>65.142857142857139</v>
       </c>
       <c r="E25" s="52">
-        <f t="shared" si="3"/>
-        <v>59.71428571</v>
+        <f t="shared" si="2"/>
+        <v>59.714285714285708</v>
       </c>
       <c r="F25" s="52">
-        <f t="shared" si="3"/>
-        <v>54.28571429</v>
+        <f t="shared" si="2"/>
+        <v>54.285714285714278</v>
       </c>
       <c r="G25" s="52">
-        <f t="shared" si="3"/>
-        <v>48.85714286</v>
+        <f t="shared" si="2"/>
+        <v>48.857142857142847</v>
       </c>
       <c r="H25" s="52">
-        <f t="shared" si="3"/>
-        <v>43.42857143</v>
+        <f t="shared" si="2"/>
+        <v>43.428571428571416</v>
       </c>
       <c r="I25" s="52">
-        <f t="shared" si="3"/>
-        <v>38</v>
+        <f t="shared" si="2"/>
+        <v>37.999999999999986</v>
       </c>
       <c r="J25" s="52">
-        <f t="shared" si="3"/>
-        <v>32.57142857</v>
+        <f t="shared" si="2"/>
+        <v>32.571428571428555</v>
       </c>
       <c r="K25" s="52">
-        <f t="shared" si="3"/>
-        <v>27.14285714</v>
+        <f t="shared" si="2"/>
+        <v>27.142857142857125</v>
       </c>
       <c r="L25" s="52">
-        <f t="shared" si="3"/>
-        <v>21.71428571</v>
+        <f t="shared" si="2"/>
+        <v>21.714285714285694</v>
       </c>
       <c r="M25" s="52">
-        <f t="shared" si="3"/>
-        <v>16.28571429</v>
+        <f t="shared" si="2"/>
+        <v>16.285714285714263</v>
       </c>
       <c r="N25" s="54">
-        <f t="shared" si="3"/>
-        <v>10.85714286</v>
+        <f t="shared" si="2"/>
+        <v>10.857142857142835</v>
       </c>
       <c r="O25" s="52">
-        <f t="shared" si="3"/>
-        <v>5.428571429</v>
+        <f t="shared" si="2"/>
+        <v>5.4285714285714057</v>
       </c>
       <c r="P25" s="52">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>-2.3092638912203256E-14</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:16" ht="15">
       <c r="A26" s="55" t="s">
         <v>31</v>
       </c>
@@ -1659,68 +2674,84 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:16" ht="15">
       <c r="A27" s="55" t="s">
         <v>32</v>
       </c>
       <c r="B27" s="7">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C27" s="7">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D27" s="7">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E27" s="7">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="F27" s="7">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G27" s="7">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="H27" s="7">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="I27" s="7">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="J27" s="7">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="K27" s="7">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="L27" s="7">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="M27" s="7">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="N27" s="7">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="O27" s="7">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="P27" s="7">
-        <v>13.0</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adding tab for sprint 5
</commit_message>
<xml_diff>
--- a/Project Management/BurnDown Charts/BurnDown Chart.xlsx
+++ b/Project Management/BurnDown Charts/BurnDown Chart.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="0" windowWidth="25600" windowHeight="15620" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="0" windowWidth="25600" windowHeight="15620" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Table Sprint 4" sheetId="1" r:id="rId1"/>
     <sheet name="Sprint 4 Chart" sheetId="2" r:id="rId2"/>
+    <sheet name="Table Sprint 5" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -680,7 +681,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -930,8 +930,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2047056680"/>
-        <c:axId val="-2114617528"/>
+        <c:axId val="-2100662328"/>
+        <c:axId val="2089607160"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1182,11 +1182,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2047056680"/>
-        <c:axId val="-2114617528"/>
+        <c:axId val="-2100662328"/>
+        <c:axId val="2089607160"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2047056680"/>
+        <c:axId val="-2100662328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1195,7 +1195,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2114617528"/>
+        <c:crossAx val="2089607160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1203,7 +1203,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2114617528"/>
+        <c:axId val="2089607160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1214,14 +1214,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2047056680"/>
+        <c:crossAx val="-2100662328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1597,7 +1596,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
@@ -2754,4 +2753,21 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added table content for sprint 5
</commit_message>
<xml_diff>
--- a/Project Management/BurnDown Charts/BurnDown Chart.xlsx
+++ b/Project Management/BurnDown Charts/BurnDown Chart.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="0" windowWidth="25600" windowHeight="15620" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="1080" windowWidth="25600" windowHeight="14980" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Table Sprint 4" sheetId="1" r:id="rId1"/>
-    <sheet name="Sprint 4 Chart" sheetId="2" r:id="rId2"/>
-    <sheet name="Table Sprint 5" sheetId="3" r:id="rId3"/>
+    <sheet name="Table Sprint 5" sheetId="2" r:id="rId2"/>
+    <sheet name="Sprint 4 Chart" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
   <si>
     <t>Stories for the Sprint 4</t>
   </si>
@@ -121,12 +121,15 @@
   <si>
     <t>Stories Completed</t>
   </si>
+  <si>
+    <t>Stories for the Sprint 5</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -157,18 +160,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Inconsolata"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color theme="10"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color theme="11"/>
-      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="9">
@@ -239,6 +230,17 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -381,17 +383,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
@@ -469,20 +460,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -502,53 +483,49 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -557,14 +534,36 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -575,6 +574,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -600,13 +602,13 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -633,17 +635,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="11">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -930,8 +922,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2100662328"/>
-        <c:axId val="2089607160"/>
+        <c:axId val="2097240744"/>
+        <c:axId val="2097237608"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1182,11 +1174,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2100662328"/>
-        <c:axId val="2089607160"/>
+        <c:axId val="2097240744"/>
+        <c:axId val="2097237608"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2100662328"/>
+        <c:axId val="2097240744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1195,7 +1187,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2089607160"/>
+        <c:crossAx val="2097237608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1203,7 +1195,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2089607160"/>
+        <c:axId val="2097237608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1214,7 +1206,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2100662328"/>
+        <c:crossAx val="2097240744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1240,19 +1232,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>914401</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:colOff>990600</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>1003301</xdr:colOff>
+      <xdr:colOff>1079500</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -1596,9 +1588,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
@@ -1659,7 +1649,7 @@
       <c r="A2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="7">
         <f t="shared" ref="B2:B14" si="0">SUM(C2:P2)</f>
         <v>3</v>
       </c>
@@ -1681,7 +1671,7 @@
       <c r="H2" s="6">
         <v>0</v>
       </c>
-      <c r="I2" s="7">
+      <c r="I2" s="9">
         <v>3</v>
       </c>
       <c r="J2" s="6">
@@ -1710,7 +1700,7 @@
       <c r="A3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="7">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
@@ -1720,7 +1710,7 @@
       <c r="D3" s="6">
         <v>2</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="9">
         <v>3</v>
       </c>
       <c r="F3" s="6">
@@ -1758,112 +1748,112 @@
       </c>
     </row>
     <row r="4" spans="1:16" ht="15">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="7">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C4" s="9">
-        <v>0</v>
-      </c>
-      <c r="D4" s="9">
-        <v>0</v>
-      </c>
-      <c r="E4" s="9">
-        <v>0</v>
-      </c>
-      <c r="F4" s="9">
-        <v>0</v>
-      </c>
-      <c r="G4" s="9">
-        <v>0</v>
-      </c>
-      <c r="H4" s="9">
-        <v>0</v>
-      </c>
-      <c r="I4" s="9">
-        <v>0</v>
-      </c>
-      <c r="J4" s="9">
-        <v>0</v>
-      </c>
-      <c r="K4" s="9">
-        <v>0</v>
-      </c>
-      <c r="L4" s="9">
-        <v>0</v>
-      </c>
-      <c r="M4" s="9">
-        <v>0</v>
-      </c>
-      <c r="N4" s="9">
+      <c r="C4" s="11">
+        <v>0</v>
+      </c>
+      <c r="D4" s="11">
+        <v>0</v>
+      </c>
+      <c r="E4" s="11">
+        <v>0</v>
+      </c>
+      <c r="F4" s="11">
+        <v>0</v>
+      </c>
+      <c r="G4" s="11">
+        <v>0</v>
+      </c>
+      <c r="H4" s="11">
+        <v>0</v>
+      </c>
+      <c r="I4" s="11">
+        <v>0</v>
+      </c>
+      <c r="J4" s="11">
+        <v>0</v>
+      </c>
+      <c r="K4" s="11">
+        <v>0</v>
+      </c>
+      <c r="L4" s="11">
+        <v>0</v>
+      </c>
+      <c r="M4" s="11">
+        <v>0</v>
+      </c>
+      <c r="N4" s="11">
         <v>3</v>
       </c>
-      <c r="O4" s="10">
+      <c r="O4" s="13">
         <v>1</v>
       </c>
-      <c r="P4" s="11">
+      <c r="P4" s="12">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="15">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="7">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="11">
         <v>1</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="11">
         <v>1</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="11">
         <v>3</v>
       </c>
-      <c r="F5" s="9">
-        <v>0</v>
-      </c>
-      <c r="G5" s="9">
-        <v>0</v>
-      </c>
-      <c r="H5" s="9">
+      <c r="F5" s="11">
+        <v>0</v>
+      </c>
+      <c r="G5" s="11">
+        <v>0</v>
+      </c>
+      <c r="H5" s="11">
         <v>2</v>
       </c>
-      <c r="I5" s="9">
+      <c r="I5" s="11">
         <v>2</v>
       </c>
-      <c r="J5" s="9">
-        <v>0</v>
-      </c>
-      <c r="K5" s="9">
-        <v>0</v>
-      </c>
-      <c r="L5" s="9">
-        <v>0</v>
-      </c>
-      <c r="M5" s="9">
+      <c r="J5" s="11">
+        <v>0</v>
+      </c>
+      <c r="K5" s="11">
+        <v>0</v>
+      </c>
+      <c r="L5" s="11">
+        <v>0</v>
+      </c>
+      <c r="M5" s="11">
         <v>1</v>
       </c>
-      <c r="N5" s="10">
+      <c r="N5" s="13">
         <v>1</v>
       </c>
-      <c r="O5" s="9">
-        <v>0</v>
-      </c>
-      <c r="P5" s="11">
+      <c r="O5" s="11">
+        <v>0</v>
+      </c>
+      <c r="P5" s="12">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="15">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="7">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
@@ -1901,367 +1891,367 @@
       <c r="N6" s="6">
         <v>3</v>
       </c>
-      <c r="O6" s="7">
+      <c r="O6" s="9">
         <v>1</v>
       </c>
-      <c r="P6" s="13">
+      <c r="P6" s="15">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="15">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="7">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C7" s="14">
-        <v>0</v>
-      </c>
-      <c r="D7" s="14">
-        <v>0</v>
-      </c>
-      <c r="E7" s="14">
-        <v>0</v>
-      </c>
-      <c r="F7" s="14">
-        <v>0</v>
-      </c>
-      <c r="G7" s="14">
-        <v>0</v>
-      </c>
-      <c r="H7" s="14">
-        <v>0</v>
-      </c>
-      <c r="I7" s="14">
-        <v>0</v>
-      </c>
-      <c r="J7" s="14">
-        <v>0</v>
-      </c>
-      <c r="K7" s="14">
-        <v>0</v>
-      </c>
-      <c r="L7" s="14">
-        <v>0</v>
-      </c>
-      <c r="M7" s="14">
-        <v>0</v>
-      </c>
-      <c r="N7" s="15">
+      <c r="C7" s="16">
+        <v>0</v>
+      </c>
+      <c r="D7" s="16">
+        <v>0</v>
+      </c>
+      <c r="E7" s="16">
+        <v>0</v>
+      </c>
+      <c r="F7" s="16">
+        <v>0</v>
+      </c>
+      <c r="G7" s="16">
+        <v>0</v>
+      </c>
+      <c r="H7" s="16">
+        <v>0</v>
+      </c>
+      <c r="I7" s="16">
+        <v>0</v>
+      </c>
+      <c r="J7" s="16">
+        <v>0</v>
+      </c>
+      <c r="K7" s="16">
+        <v>0</v>
+      </c>
+      <c r="L7" s="16">
+        <v>0</v>
+      </c>
+      <c r="M7" s="16">
+        <v>0</v>
+      </c>
+      <c r="N7" s="18">
         <v>1</v>
       </c>
-      <c r="O7" s="14">
-        <v>0</v>
-      </c>
-      <c r="P7" s="16">
+      <c r="O7" s="16">
+        <v>0</v>
+      </c>
+      <c r="P7" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="30">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="18">
+      <c r="B8" s="21">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C8" s="19">
+      <c r="C8" s="23">
         <v>2</v>
       </c>
-      <c r="D8" s="19">
+      <c r="D8" s="23">
         <v>2</v>
       </c>
-      <c r="E8" s="20">
+      <c r="E8" s="25">
         <v>2</v>
       </c>
-      <c r="F8" s="21">
-        <v>0</v>
-      </c>
-      <c r="G8" s="21">
-        <v>0</v>
-      </c>
-      <c r="H8" s="21">
-        <v>0</v>
-      </c>
-      <c r="I8" s="21">
-        <v>0</v>
-      </c>
-      <c r="J8" s="21">
-        <v>0</v>
-      </c>
-      <c r="K8" s="21">
-        <v>0</v>
-      </c>
-      <c r="L8" s="21">
-        <v>0</v>
-      </c>
-      <c r="M8" s="21">
-        <v>0</v>
-      </c>
-      <c r="N8" s="21">
-        <v>0</v>
-      </c>
-      <c r="O8" s="21">
-        <v>0</v>
-      </c>
-      <c r="P8" s="21">
+      <c r="F8" s="24">
+        <v>0</v>
+      </c>
+      <c r="G8" s="24">
+        <v>0</v>
+      </c>
+      <c r="H8" s="24">
+        <v>0</v>
+      </c>
+      <c r="I8" s="24">
+        <v>0</v>
+      </c>
+      <c r="J8" s="24">
+        <v>0</v>
+      </c>
+      <c r="K8" s="24">
+        <v>0</v>
+      </c>
+      <c r="L8" s="24">
+        <v>0</v>
+      </c>
+      <c r="M8" s="24">
+        <v>0</v>
+      </c>
+      <c r="N8" s="24">
+        <v>0</v>
+      </c>
+      <c r="O8" s="24">
+        <v>0</v>
+      </c>
+      <c r="P8" s="24">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="15">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="23">
+      <c r="B9" s="28">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C9" s="24">
-        <v>0</v>
-      </c>
-      <c r="D9" s="24">
-        <v>0</v>
-      </c>
-      <c r="E9" s="24">
-        <v>0</v>
-      </c>
-      <c r="F9" s="25">
-        <v>0</v>
-      </c>
-      <c r="G9" s="25">
-        <v>0</v>
-      </c>
-      <c r="H9" s="25">
+      <c r="C9" s="8">
+        <v>0</v>
+      </c>
+      <c r="D9" s="8">
+        <v>0</v>
+      </c>
+      <c r="E9" s="8">
+        <v>0</v>
+      </c>
+      <c r="F9" s="29">
+        <v>0</v>
+      </c>
+      <c r="G9" s="29">
+        <v>0</v>
+      </c>
+      <c r="H9" s="29">
         <v>2</v>
       </c>
-      <c r="I9" s="25">
+      <c r="I9" s="29">
         <v>3</v>
       </c>
-      <c r="J9" s="25">
-        <v>0</v>
-      </c>
-      <c r="K9" s="25">
-        <v>0</v>
-      </c>
-      <c r="L9" s="25">
-        <v>0</v>
-      </c>
-      <c r="M9" s="25">
-        <v>0</v>
-      </c>
-      <c r="N9" s="26">
+      <c r="J9" s="29">
+        <v>0</v>
+      </c>
+      <c r="K9" s="29">
+        <v>0</v>
+      </c>
+      <c r="L9" s="29">
+        <v>0</v>
+      </c>
+      <c r="M9" s="29">
+        <v>0</v>
+      </c>
+      <c r="N9" s="31">
         <v>1</v>
       </c>
-      <c r="O9" s="25">
-        <v>0</v>
-      </c>
-      <c r="P9" s="25">
+      <c r="O9" s="29">
+        <v>0</v>
+      </c>
+      <c r="P9" s="29">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="15">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="23">
+      <c r="B10" s="28">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="C10" s="24">
-        <v>0</v>
-      </c>
-      <c r="D10" s="24">
-        <v>0</v>
-      </c>
-      <c r="E10" s="24">
-        <v>0</v>
-      </c>
-      <c r="F10" s="24">
-        <v>0</v>
-      </c>
-      <c r="G10" s="24">
-        <v>0</v>
-      </c>
-      <c r="H10" s="24">
-        <v>0</v>
-      </c>
-      <c r="I10" s="24">
-        <v>0</v>
-      </c>
-      <c r="J10" s="24">
-        <v>0</v>
-      </c>
-      <c r="K10" s="24">
-        <v>0</v>
-      </c>
-      <c r="L10" s="24">
+      <c r="C10" s="8">
+        <v>0</v>
+      </c>
+      <c r="D10" s="8">
+        <v>0</v>
+      </c>
+      <c r="E10" s="8">
+        <v>0</v>
+      </c>
+      <c r="F10" s="8">
+        <v>0</v>
+      </c>
+      <c r="G10" s="8">
+        <v>0</v>
+      </c>
+      <c r="H10" s="8">
+        <v>0</v>
+      </c>
+      <c r="I10" s="8">
+        <v>0</v>
+      </c>
+      <c r="J10" s="8">
+        <v>0</v>
+      </c>
+      <c r="K10" s="8">
+        <v>0</v>
+      </c>
+      <c r="L10" s="8">
         <v>7</v>
       </c>
-      <c r="M10" s="24">
+      <c r="M10" s="8">
         <v>6</v>
       </c>
-      <c r="N10" s="27">
+      <c r="N10" s="32">
         <v>8</v>
       </c>
-      <c r="O10" s="24">
-        <v>0</v>
-      </c>
-      <c r="P10" s="24">
+      <c r="O10" s="8">
+        <v>0</v>
+      </c>
+      <c r="P10" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="15">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="23">
+      <c r="B11" s="28">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C11" s="24">
-        <v>0</v>
-      </c>
-      <c r="D11" s="24">
-        <v>0</v>
-      </c>
-      <c r="E11" s="24">
-        <v>0</v>
-      </c>
-      <c r="F11" s="24">
-        <v>0</v>
-      </c>
-      <c r="G11" s="24">
-        <v>0</v>
-      </c>
-      <c r="H11" s="24">
-        <v>0</v>
-      </c>
-      <c r="I11" s="24">
-        <v>0</v>
-      </c>
-      <c r="J11" s="24">
-        <v>0</v>
-      </c>
-      <c r="K11" s="24">
-        <v>0</v>
-      </c>
-      <c r="L11" s="27">
+      <c r="C11" s="8">
+        <v>0</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0</v>
+      </c>
+      <c r="E11" s="8">
+        <v>0</v>
+      </c>
+      <c r="F11" s="8">
+        <v>0</v>
+      </c>
+      <c r="G11" s="8">
+        <v>0</v>
+      </c>
+      <c r="H11" s="8">
+        <v>0</v>
+      </c>
+      <c r="I11" s="8">
+        <v>0</v>
+      </c>
+      <c r="J11" s="8">
+        <v>0</v>
+      </c>
+      <c r="K11" s="8">
+        <v>0</v>
+      </c>
+      <c r="L11" s="32">
         <v>1</v>
       </c>
-      <c r="M11" s="24">
-        <v>0</v>
-      </c>
-      <c r="N11" s="24">
-        <v>0</v>
-      </c>
-      <c r="O11" s="24">
-        <v>0</v>
-      </c>
-      <c r="P11" s="24">
+      <c r="M11" s="8">
+        <v>0</v>
+      </c>
+      <c r="N11" s="8">
+        <v>0</v>
+      </c>
+      <c r="O11" s="8">
+        <v>0</v>
+      </c>
+      <c r="P11" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="15">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="29">
+      <c r="B12" s="35">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C12" s="30">
-        <v>0</v>
-      </c>
-      <c r="D12" s="30">
-        <v>0</v>
-      </c>
-      <c r="E12" s="30">
-        <v>0</v>
-      </c>
-      <c r="F12" s="30">
-        <v>0</v>
-      </c>
-      <c r="G12" s="30">
-        <v>0</v>
-      </c>
-      <c r="H12" s="30">
-        <v>0</v>
-      </c>
-      <c r="I12" s="30">
-        <v>0</v>
-      </c>
-      <c r="J12" s="30">
-        <v>0</v>
-      </c>
-      <c r="K12" s="30">
-        <v>0</v>
-      </c>
-      <c r="L12" s="31">
+      <c r="C12" s="36">
+        <v>0</v>
+      </c>
+      <c r="D12" s="36">
+        <v>0</v>
+      </c>
+      <c r="E12" s="36">
+        <v>0</v>
+      </c>
+      <c r="F12" s="36">
+        <v>0</v>
+      </c>
+      <c r="G12" s="36">
+        <v>0</v>
+      </c>
+      <c r="H12" s="36">
+        <v>0</v>
+      </c>
+      <c r="I12" s="36">
+        <v>0</v>
+      </c>
+      <c r="J12" s="36">
+        <v>0</v>
+      </c>
+      <c r="K12" s="36">
+        <v>0</v>
+      </c>
+      <c r="L12" s="37">
         <v>1</v>
       </c>
-      <c r="M12" s="30">
-        <v>0</v>
-      </c>
-      <c r="N12" s="30">
-        <v>0</v>
-      </c>
-      <c r="O12" s="30">
-        <v>0</v>
-      </c>
-      <c r="P12" s="30">
+      <c r="M12" s="36">
+        <v>0</v>
+      </c>
+      <c r="N12" s="36">
+        <v>0</v>
+      </c>
+      <c r="O12" s="36">
+        <v>0</v>
+      </c>
+      <c r="P12" s="36">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="15">
-      <c r="A13" s="32" t="s">
+      <c r="A13" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="33">
+      <c r="B13" s="40">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C13" s="34">
-        <v>0</v>
-      </c>
-      <c r="D13" s="34">
-        <v>0</v>
-      </c>
-      <c r="E13" s="34">
-        <v>0</v>
-      </c>
-      <c r="F13" s="34">
-        <v>0</v>
-      </c>
-      <c r="G13" s="34">
-        <v>0</v>
-      </c>
-      <c r="H13" s="34">
-        <v>0</v>
-      </c>
-      <c r="I13" s="34">
-        <v>0</v>
-      </c>
-      <c r="J13" s="34">
-        <v>0</v>
-      </c>
-      <c r="K13" s="34">
-        <v>0</v>
-      </c>
-      <c r="L13" s="35">
+      <c r="C13" s="41">
+        <v>0</v>
+      </c>
+      <c r="D13" s="41">
+        <v>0</v>
+      </c>
+      <c r="E13" s="41">
+        <v>0</v>
+      </c>
+      <c r="F13" s="41">
+        <v>0</v>
+      </c>
+      <c r="G13" s="41">
+        <v>0</v>
+      </c>
+      <c r="H13" s="41">
+        <v>0</v>
+      </c>
+      <c r="I13" s="41">
+        <v>0</v>
+      </c>
+      <c r="J13" s="41">
+        <v>0</v>
+      </c>
+      <c r="K13" s="41">
+        <v>0</v>
+      </c>
+      <c r="L13" s="42">
         <v>1</v>
       </c>
-      <c r="M13" s="34">
-        <v>0</v>
-      </c>
-      <c r="N13" s="34">
-        <v>0</v>
-      </c>
-      <c r="O13" s="34">
-        <v>0</v>
-      </c>
-      <c r="P13" s="34">
+      <c r="M13" s="41">
+        <v>0</v>
+      </c>
+      <c r="N13" s="41">
+        <v>0</v>
+      </c>
+      <c r="O13" s="41">
+        <v>0</v>
+      </c>
+      <c r="P13" s="41">
         <v>0</v>
       </c>
     </row>
@@ -2269,7 +2259,7 @@
       <c r="A14" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="7">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
@@ -2303,7 +2293,7 @@
       <c r="L14" s="6">
         <v>0</v>
       </c>
-      <c r="M14" s="7">
+      <c r="M14" s="9">
         <v>2</v>
       </c>
       <c r="N14" s="6">
@@ -2317,415 +2307,414 @@
       </c>
     </row>
     <row r="15" spans="1:16" ht="15">
-      <c r="A15" s="36"/>
-      <c r="B15" s="29"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="37"/>
-      <c r="I15" s="37"/>
-      <c r="J15" s="37"/>
-      <c r="K15" s="37"/>
-      <c r="L15" s="37"/>
-      <c r="M15" s="37"/>
-      <c r="N15" s="37"/>
-      <c r="O15" s="37"/>
-      <c r="P15" s="37"/>
+      <c r="A15" s="43"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="44"/>
+      <c r="J15" s="44"/>
+      <c r="K15" s="44"/>
+      <c r="L15" s="44"/>
+      <c r="M15" s="44"/>
+      <c r="N15" s="44"/>
+      <c r="O15" s="44"/>
+      <c r="P15" s="44"/>
     </row>
     <row r="16" spans="1:16" ht="15">
-      <c r="A16" s="38"/>
-      <c r="B16" s="39"/>
-      <c r="C16" s="40"/>
-      <c r="D16" s="40"/>
-      <c r="E16" s="40"/>
-      <c r="F16" s="40"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="40"/>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
-      <c r="K16" s="40"/>
-      <c r="L16" s="40"/>
-      <c r="M16" s="40"/>
-      <c r="N16" s="40"/>
-      <c r="O16" s="40"/>
-      <c r="P16" s="40"/>
+      <c r="A16" s="45"/>
+      <c r="B16" s="46"/>
+      <c r="C16" s="47"/>
+      <c r="D16" s="47"/>
+      <c r="E16" s="47"/>
+      <c r="F16" s="47"/>
+      <c r="G16" s="47"/>
+      <c r="H16" s="47"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="47"/>
+      <c r="K16" s="47"/>
+      <c r="L16" s="47"/>
+      <c r="M16" s="47"/>
+      <c r="N16" s="47"/>
+      <c r="O16" s="47"/>
+      <c r="P16" s="47"/>
     </row>
     <row r="17" spans="1:16" ht="15">
-      <c r="A17" s="38"/>
-      <c r="B17" s="39"/>
-      <c r="C17" s="41"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="41"/>
-      <c r="H17" s="41"/>
-      <c r="I17" s="41"/>
-      <c r="J17" s="41"/>
-      <c r="K17" s="41"/>
-      <c r="L17" s="41"/>
-      <c r="M17" s="41"/>
-      <c r="N17" s="41"/>
-      <c r="O17" s="40"/>
-      <c r="P17" s="40"/>
+      <c r="A17" s="45"/>
+      <c r="B17" s="46"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="48"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="48"/>
+      <c r="I17" s="48"/>
+      <c r="J17" s="48"/>
+      <c r="K17" s="48"/>
+      <c r="L17" s="48"/>
+      <c r="M17" s="48"/>
+      <c r="N17" s="48"/>
+      <c r="O17" s="47"/>
+      <c r="P17" s="47"/>
     </row>
     <row r="18" spans="1:16" ht="15">
-      <c r="A18" s="38"/>
-      <c r="B18" s="42"/>
-      <c r="C18" s="43"/>
-      <c r="D18" s="43"/>
-      <c r="E18" s="43"/>
-      <c r="F18" s="43"/>
-      <c r="G18" s="43"/>
-      <c r="H18" s="43"/>
-      <c r="I18" s="43"/>
-      <c r="J18" s="43"/>
-      <c r="K18" s="43"/>
-      <c r="L18" s="43"/>
-      <c r="M18" s="43"/>
-      <c r="N18" s="43"/>
-      <c r="O18" s="40"/>
-      <c r="P18" s="40"/>
+      <c r="A18" s="45"/>
+      <c r="B18" s="49"/>
+      <c r="C18" s="50"/>
+      <c r="D18" s="50"/>
+      <c r="E18" s="50"/>
+      <c r="F18" s="50"/>
+      <c r="G18" s="50"/>
+      <c r="H18" s="50"/>
+      <c r="I18" s="50"/>
+      <c r="J18" s="50"/>
+      <c r="K18" s="50"/>
+      <c r="L18" s="50"/>
+      <c r="M18" s="50"/>
+      <c r="N18" s="50"/>
+      <c r="O18" s="47"/>
+      <c r="P18" s="47"/>
     </row>
     <row r="19" spans="1:16" ht="15">
       <c r="A19" s="4"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="44"/>
-      <c r="D19" s="44"/>
-      <c r="E19" s="44"/>
-      <c r="F19" s="44"/>
-      <c r="G19" s="44"/>
-      <c r="H19" s="44"/>
-      <c r="I19" s="44"/>
-      <c r="J19" s="44"/>
-      <c r="K19" s="44"/>
-      <c r="L19" s="44"/>
-      <c r="M19" s="44"/>
-      <c r="N19" s="44"/>
-      <c r="O19" s="44"/>
-      <c r="P19" s="44"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="51"/>
+      <c r="D19" s="51"/>
+      <c r="E19" s="51"/>
+      <c r="F19" s="51"/>
+      <c r="G19" s="51"/>
+      <c r="H19" s="51"/>
+      <c r="I19" s="51"/>
+      <c r="J19" s="51"/>
+      <c r="K19" s="51"/>
+      <c r="L19" s="51"/>
+      <c r="M19" s="51"/>
+      <c r="N19" s="51"/>
+      <c r="O19" s="51"/>
+      <c r="P19" s="51"/>
     </row>
     <row r="20" spans="1:16" ht="15">
-      <c r="A20" s="45"/>
-      <c r="B20" s="46"/>
-      <c r="C20" s="47"/>
-      <c r="D20" s="47"/>
-      <c r="E20" s="47"/>
-      <c r="F20" s="47"/>
-      <c r="G20" s="47"/>
-      <c r="H20" s="47"/>
-      <c r="I20" s="47"/>
-      <c r="J20" s="47"/>
-      <c r="K20" s="47"/>
-      <c r="L20" s="47"/>
-      <c r="M20" s="47"/>
-      <c r="N20" s="47"/>
-      <c r="O20" s="47"/>
-      <c r="P20" s="47"/>
+      <c r="A20" s="52"/>
+      <c r="B20" s="53"/>
+      <c r="C20" s="54"/>
+      <c r="D20" s="54"/>
+      <c r="E20" s="54"/>
+      <c r="F20" s="54"/>
+      <c r="G20" s="54"/>
+      <c r="H20" s="54"/>
+      <c r="I20" s="54"/>
+      <c r="J20" s="54"/>
+      <c r="K20" s="54"/>
+      <c r="L20" s="54"/>
+      <c r="M20" s="54"/>
+      <c r="N20" s="54"/>
+      <c r="O20" s="54"/>
+      <c r="P20" s="54"/>
     </row>
     <row r="21" spans="1:16" ht="15">
       <c r="A21" s="4"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="44"/>
-      <c r="D21" s="44"/>
-      <c r="E21" s="44"/>
-      <c r="F21" s="44"/>
-      <c r="G21" s="44"/>
-      <c r="H21" s="44"/>
-      <c r="I21" s="44"/>
-      <c r="J21" s="44"/>
-      <c r="K21" s="44"/>
-      <c r="L21" s="44"/>
-      <c r="M21" s="44"/>
-      <c r="N21" s="44"/>
-      <c r="O21" s="44"/>
-      <c r="P21" s="44"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="51"/>
+      <c r="D21" s="51"/>
+      <c r="E21" s="51"/>
+      <c r="F21" s="51"/>
+      <c r="G21" s="51"/>
+      <c r="H21" s="51"/>
+      <c r="I21" s="51"/>
+      <c r="J21" s="51"/>
+      <c r="K21" s="51"/>
+      <c r="L21" s="51"/>
+      <c r="M21" s="51"/>
+      <c r="N21" s="51"/>
+      <c r="O21" s="51"/>
+      <c r="P21" s="51"/>
     </row>
     <row r="22" spans="1:16" ht="15">
-      <c r="A22" s="48"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="49"/>
-      <c r="D22" s="49"/>
-      <c r="E22" s="49"/>
-      <c r="F22" s="49"/>
-      <c r="G22" s="49"/>
-      <c r="H22" s="49"/>
-      <c r="I22" s="49"/>
-      <c r="J22" s="49"/>
-      <c r="K22" s="49"/>
-      <c r="L22" s="49"/>
-      <c r="M22" s="49"/>
-      <c r="N22" s="49"/>
-      <c r="O22" s="49"/>
-      <c r="P22" s="49"/>
+      <c r="A22" s="55"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="56"/>
+      <c r="D22" s="56"/>
+      <c r="E22" s="56"/>
+      <c r="F22" s="56"/>
+      <c r="G22" s="56"/>
+      <c r="H22" s="56"/>
+      <c r="I22" s="56"/>
+      <c r="J22" s="56"/>
+      <c r="K22" s="56"/>
+      <c r="L22" s="56"/>
+      <c r="M22" s="56"/>
+      <c r="N22" s="56"/>
+      <c r="O22" s="56"/>
+      <c r="P22" s="56"/>
     </row>
     <row r="23" spans="1:16" ht="15">
-      <c r="A23" s="48"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="50"/>
-      <c r="D23" s="50"/>
-      <c r="E23" s="50"/>
-      <c r="F23" s="50"/>
-      <c r="G23" s="50"/>
-      <c r="H23" s="50"/>
-      <c r="I23" s="50"/>
-      <c r="J23" s="50"/>
-      <c r="K23" s="50"/>
-      <c r="L23" s="50"/>
-      <c r="M23" s="50"/>
-      <c r="N23" s="50"/>
-      <c r="O23" s="50"/>
-      <c r="P23" s="50"/>
+      <c r="A23" s="55"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="57"/>
+      <c r="D23" s="57"/>
+      <c r="E23" s="57"/>
+      <c r="F23" s="57"/>
+      <c r="G23" s="57"/>
+      <c r="H23" s="57"/>
+      <c r="I23" s="57"/>
+      <c r="J23" s="57"/>
+      <c r="K23" s="57"/>
+      <c r="L23" s="57"/>
+      <c r="M23" s="57"/>
+      <c r="N23" s="57"/>
+      <c r="O23" s="57"/>
+      <c r="P23" s="57"/>
     </row>
     <row r="24" spans="1:16" ht="15">
-      <c r="A24" s="51" t="s">
+      <c r="A24" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="52">
+      <c r="B24" s="59">
         <f>SUM(B2:B23)</f>
         <v>76</v>
       </c>
-      <c r="C24" s="52">
+      <c r="C24" s="59">
         <f t="shared" ref="C24:P24" si="1">SUM(B24-SUM(C2:C23))</f>
         <v>71</v>
       </c>
-      <c r="D24" s="52">
+      <c r="D24" s="59">
         <f t="shared" si="1"/>
         <v>65</v>
       </c>
-      <c r="E24" s="52">
+      <c r="E24" s="59">
         <f t="shared" si="1"/>
         <v>57</v>
       </c>
-      <c r="F24" s="52">
+      <c r="F24" s="59">
         <f t="shared" si="1"/>
         <v>57</v>
       </c>
-      <c r="G24" s="52">
+      <c r="G24" s="59">
         <f t="shared" si="1"/>
         <v>57</v>
       </c>
-      <c r="H24" s="52">
+      <c r="H24" s="59">
         <f t="shared" si="1"/>
         <v>53</v>
       </c>
-      <c r="I24" s="52">
+      <c r="I24" s="59">
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="J24" s="52">
+      <c r="J24" s="59">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="K24" s="52">
+      <c r="K24" s="59">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="L24" s="52">
+      <c r="L24" s="59">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="M24" s="52">
+      <c r="M24" s="59">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="N24" s="53">
+      <c r="N24" s="60">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="O24" s="52">
+      <c r="O24" s="59">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P24" s="52">
+      <c r="P24" s="59">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="15">
-      <c r="A25" s="51" t="s">
+      <c r="A25" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="B25" s="52">
+      <c r="B25" s="59">
         <f>B24</f>
         <v>76</v>
       </c>
-      <c r="C25" s="52">
+      <c r="C25" s="59">
         <f t="shared" ref="C25:P25" si="2">B25-$B25/14</f>
         <v>70.571428571428569</v>
       </c>
-      <c r="D25" s="52">
+      <c r="D25" s="59">
         <f t="shared" si="2"/>
         <v>65.142857142857139</v>
       </c>
-      <c r="E25" s="52">
+      <c r="E25" s="59">
         <f t="shared" si="2"/>
         <v>59.714285714285708</v>
       </c>
-      <c r="F25" s="52">
+      <c r="F25" s="59">
         <f t="shared" si="2"/>
         <v>54.285714285714278</v>
       </c>
-      <c r="G25" s="52">
+      <c r="G25" s="59">
         <f t="shared" si="2"/>
         <v>48.857142857142847</v>
       </c>
-      <c r="H25" s="52">
+      <c r="H25" s="59">
         <f t="shared" si="2"/>
         <v>43.428571428571416</v>
       </c>
-      <c r="I25" s="52">
+      <c r="I25" s="59">
         <f t="shared" si="2"/>
         <v>37.999999999999986</v>
       </c>
-      <c r="J25" s="52">
+      <c r="J25" s="59">
         <f t="shared" si="2"/>
         <v>32.571428571428555</v>
       </c>
-      <c r="K25" s="52">
+      <c r="K25" s="59">
         <f t="shared" si="2"/>
         <v>27.142857142857125</v>
       </c>
-      <c r="L25" s="52">
+      <c r="L25" s="59">
         <f t="shared" si="2"/>
         <v>21.714285714285694</v>
       </c>
-      <c r="M25" s="52">
+      <c r="M25" s="59">
         <f t="shared" si="2"/>
         <v>16.285714285714263</v>
       </c>
-      <c r="N25" s="54">
+      <c r="N25" s="61">
         <f t="shared" si="2"/>
         <v>10.857142857142835</v>
       </c>
-      <c r="O25" s="52">
+      <c r="O25" s="59">
         <f t="shared" si="2"/>
         <v>5.4285714285714057</v>
       </c>
-      <c r="P25" s="52">
+      <c r="P25" s="59">
         <f t="shared" si="2"/>
         <v>-2.3092638912203256E-14</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="15">
-      <c r="A26" s="55" t="s">
+      <c r="A26" s="62" t="s">
         <v>31</v>
       </c>
-      <c r="B26" s="56">
+      <c r="B26" s="63">
         <f>ROWS(A2:A14)</f>
         <v>13</v>
       </c>
-      <c r="C26" s="56">
+      <c r="C26" s="63">
         <f>B26-C27</f>
         <v>13</v>
       </c>
-      <c r="D26" s="56">
+      <c r="D26" s="63">
         <f>B26-D27</f>
         <v>13</v>
       </c>
-      <c r="E26" s="56">
+      <c r="E26" s="63">
         <f>B26-E27</f>
         <v>11</v>
       </c>
-      <c r="F26" s="56">
+      <c r="F26" s="63">
         <f>B26-F27</f>
         <v>11</v>
       </c>
-      <c r="G26" s="56">
+      <c r="G26" s="63">
         <f>B26-G27</f>
         <v>11</v>
       </c>
-      <c r="H26" s="56">
+      <c r="H26" s="63">
         <f>B26-H27</f>
         <v>11</v>
       </c>
-      <c r="I26" s="56">
+      <c r="I26" s="63">
         <f>B26-I27</f>
         <v>10</v>
       </c>
-      <c r="J26" s="56">
+      <c r="J26" s="63">
         <f>B26-J27</f>
         <v>10</v>
       </c>
-      <c r="K26" s="56">
+      <c r="K26" s="63">
         <f>B26-K27</f>
         <v>10</v>
       </c>
-      <c r="L26" s="56">
+      <c r="L26" s="63">
         <f>B26-L27</f>
         <v>7</v>
       </c>
-      <c r="M26" s="56">
+      <c r="M26" s="63">
         <f>B26-M27</f>
         <v>6</v>
       </c>
-      <c r="N26" s="56">
+      <c r="N26" s="63">
         <f>B26-N27</f>
         <v>2</v>
       </c>
-      <c r="O26" s="56">
+      <c r="O26" s="63">
         <f>B26-O27</f>
         <v>0</v>
       </c>
-      <c r="P26" s="56">
+      <c r="P26" s="63">
         <f>B26-P27</f>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="15">
-      <c r="A27" s="55" t="s">
+      <c r="A27" s="62" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="7">
-        <v>0</v>
-      </c>
-      <c r="C27" s="7">
-        <v>0</v>
-      </c>
-      <c r="D27" s="7">
-        <v>0</v>
-      </c>
-      <c r="E27" s="7">
+      <c r="B27" s="9">
+        <v>0</v>
+      </c>
+      <c r="C27" s="9">
+        <v>0</v>
+      </c>
+      <c r="D27" s="9">
+        <v>0</v>
+      </c>
+      <c r="E27" s="9">
         <v>2</v>
       </c>
-      <c r="F27" s="7">
+      <c r="F27" s="9">
         <v>2</v>
       </c>
-      <c r="G27" s="7">
+      <c r="G27" s="9">
         <v>2</v>
       </c>
-      <c r="H27" s="7">
+      <c r="H27" s="9">
         <v>2</v>
       </c>
-      <c r="I27" s="7">
+      <c r="I27" s="9">
         <v>3</v>
       </c>
-      <c r="J27" s="7">
+      <c r="J27" s="9">
         <v>3</v>
       </c>
-      <c r="K27" s="7">
+      <c r="K27" s="9">
         <v>3</v>
       </c>
-      <c r="L27" s="7">
+      <c r="L27" s="9">
         <v>6</v>
       </c>
-      <c r="M27" s="7">
+      <c r="M27" s="9">
         <v>7</v>
       </c>
-      <c r="N27" s="7">
+      <c r="N27" s="9">
         <v>11</v>
       </c>
-      <c r="O27" s="7">
+      <c r="O27" s="9">
         <v>13</v>
       </c>
-      <c r="P27" s="7">
+      <c r="P27" s="9">
         <v>13</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2736,17 +2725,1097 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="34.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="15.75" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="15.75" customHeight="1">
+      <c r="A2" s="4"/>
+      <c r="B2" s="5">
+        <v>0</v>
+      </c>
+      <c r="C2" s="6">
+        <v>0</v>
+      </c>
+      <c r="D2" s="6">
+        <v>0</v>
+      </c>
+      <c r="E2" s="6">
+        <v>0</v>
+      </c>
+      <c r="F2" s="6">
+        <v>0</v>
+      </c>
+      <c r="G2" s="6">
+        <v>0</v>
+      </c>
+      <c r="H2" s="6">
+        <v>0</v>
+      </c>
+      <c r="I2" s="8">
+        <v>0</v>
+      </c>
+      <c r="J2" s="6">
+        <v>0</v>
+      </c>
+      <c r="K2" s="6">
+        <v>0</v>
+      </c>
+      <c r="L2" s="6">
+        <v>0</v>
+      </c>
+      <c r="M2" s="6">
+        <v>0</v>
+      </c>
+      <c r="N2" s="6">
+        <v>0</v>
+      </c>
+      <c r="O2" s="6">
+        <v>0</v>
+      </c>
+      <c r="P2" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="15.75" customHeight="1">
+      <c r="A3" s="4"/>
+      <c r="B3" s="5">
+        <v>0</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0</v>
+      </c>
+      <c r="D3" s="6">
+        <v>0</v>
+      </c>
+      <c r="E3" s="8">
+        <v>0</v>
+      </c>
+      <c r="F3" s="6">
+        <v>0</v>
+      </c>
+      <c r="G3" s="6">
+        <v>0</v>
+      </c>
+      <c r="H3" s="6">
+        <v>0</v>
+      </c>
+      <c r="I3" s="6">
+        <v>0</v>
+      </c>
+      <c r="J3" s="6">
+        <v>0</v>
+      </c>
+      <c r="K3" s="6">
+        <v>0</v>
+      </c>
+      <c r="L3" s="6">
+        <v>0</v>
+      </c>
+      <c r="M3" s="6">
+        <v>0</v>
+      </c>
+      <c r="N3" s="6">
+        <v>0</v>
+      </c>
+      <c r="O3" s="6">
+        <v>0</v>
+      </c>
+      <c r="P3" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="15.75" customHeight="1">
+      <c r="A4" s="10"/>
+      <c r="B4" s="5">
+        <v>0</v>
+      </c>
+      <c r="C4" s="11">
+        <v>0</v>
+      </c>
+      <c r="D4" s="11">
+        <v>0</v>
+      </c>
+      <c r="E4" s="11">
+        <v>0</v>
+      </c>
+      <c r="F4" s="11">
+        <v>0</v>
+      </c>
+      <c r="G4" s="11">
+        <v>0</v>
+      </c>
+      <c r="H4" s="11">
+        <v>0</v>
+      </c>
+      <c r="I4" s="11">
+        <v>0</v>
+      </c>
+      <c r="J4" s="11">
+        <v>0</v>
+      </c>
+      <c r="K4" s="11">
+        <v>0</v>
+      </c>
+      <c r="L4" s="11">
+        <v>0</v>
+      </c>
+      <c r="M4" s="11">
+        <v>0</v>
+      </c>
+      <c r="N4" s="11">
+        <v>0</v>
+      </c>
+      <c r="O4" s="8">
+        <v>0</v>
+      </c>
+      <c r="P4" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="15.75" customHeight="1">
+      <c r="A5" s="10"/>
+      <c r="B5" s="5">
+        <v>0</v>
+      </c>
+      <c r="C5" s="11">
+        <v>0</v>
+      </c>
+      <c r="D5" s="11">
+        <v>0</v>
+      </c>
+      <c r="E5" s="11">
+        <v>0</v>
+      </c>
+      <c r="F5" s="11">
+        <v>0</v>
+      </c>
+      <c r="G5" s="11">
+        <v>0</v>
+      </c>
+      <c r="H5" s="11">
+        <v>0</v>
+      </c>
+      <c r="I5" s="11">
+        <v>0</v>
+      </c>
+      <c r="J5" s="11">
+        <v>0</v>
+      </c>
+      <c r="K5" s="11">
+        <v>0</v>
+      </c>
+      <c r="L5" s="11">
+        <v>0</v>
+      </c>
+      <c r="M5" s="11">
+        <v>0</v>
+      </c>
+      <c r="N5" s="8">
+        <v>0</v>
+      </c>
+      <c r="O5" s="11">
+        <v>0</v>
+      </c>
+      <c r="P5" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="15.75" customHeight="1">
+      <c r="A6" s="14"/>
+      <c r="B6" s="5">
+        <v>0</v>
+      </c>
+      <c r="C6" s="6">
+        <v>0</v>
+      </c>
+      <c r="D6" s="6">
+        <v>0</v>
+      </c>
+      <c r="E6" s="6">
+        <v>0</v>
+      </c>
+      <c r="F6" s="6">
+        <v>0</v>
+      </c>
+      <c r="G6" s="6">
+        <v>0</v>
+      </c>
+      <c r="H6" s="6">
+        <v>0</v>
+      </c>
+      <c r="I6" s="6">
+        <v>0</v>
+      </c>
+      <c r="J6" s="6">
+        <v>0</v>
+      </c>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6">
+        <v>0</v>
+      </c>
+      <c r="M6" s="6">
+        <v>0</v>
+      </c>
+      <c r="N6" s="6">
+        <v>0</v>
+      </c>
+      <c r="O6" s="8">
+        <v>0</v>
+      </c>
+      <c r="P6" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="15.75" customHeight="1">
+      <c r="A7" s="14"/>
+      <c r="B7" s="5">
+        <v>0</v>
+      </c>
+      <c r="C7" s="16">
+        <v>0</v>
+      </c>
+      <c r="D7" s="16">
+        <v>0</v>
+      </c>
+      <c r="E7" s="16">
+        <v>0</v>
+      </c>
+      <c r="F7" s="16">
+        <v>0</v>
+      </c>
+      <c r="G7" s="16">
+        <v>0</v>
+      </c>
+      <c r="H7" s="16">
+        <v>0</v>
+      </c>
+      <c r="I7" s="16">
+        <v>0</v>
+      </c>
+      <c r="J7" s="16">
+        <v>0</v>
+      </c>
+      <c r="K7" s="16">
+        <v>0</v>
+      </c>
+      <c r="L7" s="16">
+        <v>0</v>
+      </c>
+      <c r="M7" s="16">
+        <v>0</v>
+      </c>
+      <c r="N7" s="8">
+        <v>0</v>
+      </c>
+      <c r="O7" s="16">
+        <v>0</v>
+      </c>
+      <c r="P7" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="15.75" customHeight="1">
+      <c r="A8" s="19"/>
+      <c r="B8" s="20">
+        <v>0</v>
+      </c>
+      <c r="C8" s="22">
+        <v>0</v>
+      </c>
+      <c r="D8" s="22">
+        <v>0</v>
+      </c>
+      <c r="E8" s="8">
+        <v>0</v>
+      </c>
+      <c r="F8" s="24">
+        <v>0</v>
+      </c>
+      <c r="G8" s="24">
+        <v>0</v>
+      </c>
+      <c r="H8" s="24">
+        <v>0</v>
+      </c>
+      <c r="I8" s="24">
+        <v>0</v>
+      </c>
+      <c r="J8" s="24">
+        <v>0</v>
+      </c>
+      <c r="K8" s="24">
+        <v>0</v>
+      </c>
+      <c r="L8" s="24">
+        <v>0</v>
+      </c>
+      <c r="M8" s="24">
+        <v>0</v>
+      </c>
+      <c r="N8" s="24">
+        <v>0</v>
+      </c>
+      <c r="O8" s="24">
+        <v>0</v>
+      </c>
+      <c r="P8" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="15.75" customHeight="1">
+      <c r="A9" s="26"/>
+      <c r="B9" s="27">
+        <v>0</v>
+      </c>
+      <c r="C9" s="8">
+        <v>0</v>
+      </c>
+      <c r="D9" s="8">
+        <v>0</v>
+      </c>
+      <c r="E9" s="8">
+        <v>0</v>
+      </c>
+      <c r="F9" s="29">
+        <v>0</v>
+      </c>
+      <c r="G9" s="29">
+        <v>0</v>
+      </c>
+      <c r="H9" s="30">
+        <v>0</v>
+      </c>
+      <c r="I9" s="30">
+        <v>0</v>
+      </c>
+      <c r="J9" s="29">
+        <v>0</v>
+      </c>
+      <c r="K9" s="29">
+        <v>0</v>
+      </c>
+      <c r="L9" s="29">
+        <v>0</v>
+      </c>
+      <c r="M9" s="29">
+        <v>0</v>
+      </c>
+      <c r="N9" s="8">
+        <v>0</v>
+      </c>
+      <c r="O9" s="29">
+        <v>0</v>
+      </c>
+      <c r="P9" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="15.75" customHeight="1">
+      <c r="A10" s="26"/>
+      <c r="B10" s="27">
+        <v>0</v>
+      </c>
+      <c r="C10" s="8">
+        <v>0</v>
+      </c>
+      <c r="D10" s="8">
+        <v>0</v>
+      </c>
+      <c r="E10" s="8">
+        <v>0</v>
+      </c>
+      <c r="F10" s="8">
+        <v>0</v>
+      </c>
+      <c r="G10" s="8">
+        <v>0</v>
+      </c>
+      <c r="H10" s="8">
+        <v>0</v>
+      </c>
+      <c r="I10" s="8">
+        <v>0</v>
+      </c>
+      <c r="J10" s="8">
+        <v>0</v>
+      </c>
+      <c r="K10" s="8">
+        <v>0</v>
+      </c>
+      <c r="L10" s="30">
+        <v>0</v>
+      </c>
+      <c r="M10" s="30">
+        <v>0</v>
+      </c>
+      <c r="N10" s="8">
+        <v>0</v>
+      </c>
+      <c r="O10" s="8">
+        <v>0</v>
+      </c>
+      <c r="P10" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="15.75" customHeight="1">
+      <c r="A11" s="26"/>
+      <c r="B11" s="27">
+        <v>0</v>
+      </c>
+      <c r="C11" s="8">
+        <v>0</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0</v>
+      </c>
+      <c r="E11" s="8">
+        <v>0</v>
+      </c>
+      <c r="F11" s="8">
+        <v>0</v>
+      </c>
+      <c r="G11" s="8">
+        <v>0</v>
+      </c>
+      <c r="H11" s="8">
+        <v>0</v>
+      </c>
+      <c r="I11" s="8">
+        <v>0</v>
+      </c>
+      <c r="J11" s="8">
+        <v>0</v>
+      </c>
+      <c r="K11" s="8">
+        <v>0</v>
+      </c>
+      <c r="L11" s="8">
+        <v>0</v>
+      </c>
+      <c r="M11" s="8">
+        <v>0</v>
+      </c>
+      <c r="N11" s="8">
+        <v>0</v>
+      </c>
+      <c r="O11" s="8">
+        <v>0</v>
+      </c>
+      <c r="P11" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="15.75" customHeight="1">
+      <c r="A12" s="33"/>
+      <c r="B12" s="34">
+        <v>0</v>
+      </c>
+      <c r="C12" s="36">
+        <v>0</v>
+      </c>
+      <c r="D12" s="36">
+        <v>0</v>
+      </c>
+      <c r="E12" s="36">
+        <v>0</v>
+      </c>
+      <c r="F12" s="36">
+        <v>0</v>
+      </c>
+      <c r="G12" s="36">
+        <v>0</v>
+      </c>
+      <c r="H12" s="36">
+        <v>0</v>
+      </c>
+      <c r="I12" s="36">
+        <v>0</v>
+      </c>
+      <c r="J12" s="36">
+        <v>0</v>
+      </c>
+      <c r="K12" s="36">
+        <v>0</v>
+      </c>
+      <c r="L12" s="8">
+        <v>0</v>
+      </c>
+      <c r="M12" s="36">
+        <v>0</v>
+      </c>
+      <c r="N12" s="36">
+        <v>0</v>
+      </c>
+      <c r="O12" s="36">
+        <v>0</v>
+      </c>
+      <c r="P12" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="15.75" customHeight="1">
+      <c r="A13" s="38"/>
+      <c r="B13" s="39">
+        <v>0</v>
+      </c>
+      <c r="C13" s="41">
+        <v>0</v>
+      </c>
+      <c r="D13" s="41">
+        <v>0</v>
+      </c>
+      <c r="E13" s="41">
+        <v>0</v>
+      </c>
+      <c r="F13" s="41">
+        <v>0</v>
+      </c>
+      <c r="G13" s="41">
+        <v>0</v>
+      </c>
+      <c r="H13" s="41">
+        <v>0</v>
+      </c>
+      <c r="I13" s="41">
+        <v>0</v>
+      </c>
+      <c r="J13" s="41">
+        <v>0</v>
+      </c>
+      <c r="K13" s="41">
+        <v>0</v>
+      </c>
+      <c r="L13" s="8">
+        <v>0</v>
+      </c>
+      <c r="M13" s="41">
+        <v>0</v>
+      </c>
+      <c r="N13" s="41">
+        <v>0</v>
+      </c>
+      <c r="O13" s="41">
+        <v>0</v>
+      </c>
+      <c r="P13" s="41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="15.75" customHeight="1">
+      <c r="A14" s="4"/>
+      <c r="B14" s="5">
+        <v>0</v>
+      </c>
+      <c r="C14" s="6">
+        <v>0</v>
+      </c>
+      <c r="D14" s="6">
+        <v>0</v>
+      </c>
+      <c r="E14" s="6">
+        <v>0</v>
+      </c>
+      <c r="F14" s="6">
+        <v>0</v>
+      </c>
+      <c r="G14" s="6">
+        <v>0</v>
+      </c>
+      <c r="H14" s="6">
+        <v>0</v>
+      </c>
+      <c r="I14" s="6">
+        <v>0</v>
+      </c>
+      <c r="J14" s="6">
+        <v>0</v>
+      </c>
+      <c r="K14" s="6">
+        <v>0</v>
+      </c>
+      <c r="L14" s="6">
+        <v>0</v>
+      </c>
+      <c r="M14" s="8">
+        <v>0</v>
+      </c>
+      <c r="N14" s="6">
+        <v>0</v>
+      </c>
+      <c r="O14" s="6">
+        <v>0</v>
+      </c>
+      <c r="P14" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="15.75" customHeight="1">
+      <c r="A15" s="43"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="44"/>
+      <c r="J15" s="44"/>
+      <c r="K15" s="44"/>
+      <c r="L15" s="44"/>
+      <c r="M15" s="44"/>
+      <c r="N15" s="44"/>
+      <c r="O15" s="44"/>
+      <c r="P15" s="44"/>
+    </row>
+    <row r="16" spans="1:16" ht="15.75" customHeight="1">
+      <c r="A16" s="45"/>
+      <c r="B16" s="46"/>
+      <c r="C16" s="47"/>
+      <c r="D16" s="47"/>
+      <c r="E16" s="47"/>
+      <c r="F16" s="47"/>
+      <c r="G16" s="47"/>
+      <c r="H16" s="47"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="47"/>
+      <c r="K16" s="47"/>
+      <c r="L16" s="47"/>
+      <c r="M16" s="47"/>
+      <c r="N16" s="47"/>
+      <c r="O16" s="47"/>
+      <c r="P16" s="47"/>
+    </row>
+    <row r="17" spans="1:16" ht="15.75" customHeight="1">
+      <c r="A17" s="45"/>
+      <c r="B17" s="46"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="48"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="48"/>
+      <c r="I17" s="48"/>
+      <c r="J17" s="48"/>
+      <c r="K17" s="48"/>
+      <c r="L17" s="48"/>
+      <c r="M17" s="48"/>
+      <c r="N17" s="48"/>
+      <c r="O17" s="47"/>
+      <c r="P17" s="47"/>
+    </row>
+    <row r="18" spans="1:16" ht="15.75" customHeight="1">
+      <c r="A18" s="45"/>
+      <c r="B18" s="49"/>
+      <c r="C18" s="50"/>
+      <c r="D18" s="50"/>
+      <c r="E18" s="50"/>
+      <c r="F18" s="50"/>
+      <c r="G18" s="50"/>
+      <c r="H18" s="50"/>
+      <c r="I18" s="50"/>
+      <c r="J18" s="50"/>
+      <c r="K18" s="50"/>
+      <c r="L18" s="50"/>
+      <c r="M18" s="50"/>
+      <c r="N18" s="50"/>
+      <c r="O18" s="47"/>
+      <c r="P18" s="47"/>
+    </row>
+    <row r="19" spans="1:16" ht="15.75" customHeight="1">
+      <c r="A19" s="4"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="51"/>
+      <c r="D19" s="51"/>
+      <c r="E19" s="51"/>
+      <c r="F19" s="51"/>
+      <c r="G19" s="51"/>
+      <c r="H19" s="51"/>
+      <c r="I19" s="51"/>
+      <c r="J19" s="51"/>
+      <c r="K19" s="51"/>
+      <c r="L19" s="51"/>
+      <c r="M19" s="51"/>
+      <c r="N19" s="51"/>
+      <c r="O19" s="51"/>
+      <c r="P19" s="51"/>
+    </row>
+    <row r="20" spans="1:16" ht="15.75" customHeight="1">
+      <c r="A20" s="52"/>
+      <c r="B20" s="53"/>
+      <c r="C20" s="54"/>
+      <c r="D20" s="54"/>
+      <c r="E20" s="54"/>
+      <c r="F20" s="54"/>
+      <c r="G20" s="54"/>
+      <c r="H20" s="54"/>
+      <c r="I20" s="54"/>
+      <c r="J20" s="54"/>
+      <c r="K20" s="54"/>
+      <c r="L20" s="54"/>
+      <c r="M20" s="54"/>
+      <c r="N20" s="54"/>
+      <c r="O20" s="54"/>
+      <c r="P20" s="54"/>
+    </row>
+    <row r="21" spans="1:16" ht="15.75" customHeight="1">
+      <c r="A21" s="4"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="51"/>
+      <c r="D21" s="51"/>
+      <c r="E21" s="51"/>
+      <c r="F21" s="51"/>
+      <c r="G21" s="51"/>
+      <c r="H21" s="51"/>
+      <c r="I21" s="51"/>
+      <c r="J21" s="51"/>
+      <c r="K21" s="51"/>
+      <c r="L21" s="51"/>
+      <c r="M21" s="51"/>
+      <c r="N21" s="51"/>
+      <c r="O21" s="51"/>
+      <c r="P21" s="51"/>
+    </row>
+    <row r="22" spans="1:16" ht="15.75" customHeight="1">
+      <c r="A22" s="55"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="56"/>
+      <c r="D22" s="56"/>
+      <c r="E22" s="56"/>
+      <c r="F22" s="56"/>
+      <c r="G22" s="56"/>
+      <c r="H22" s="56"/>
+      <c r="I22" s="56"/>
+      <c r="J22" s="56"/>
+      <c r="K22" s="56"/>
+      <c r="L22" s="56"/>
+      <c r="M22" s="56"/>
+      <c r="N22" s="56"/>
+      <c r="O22" s="56"/>
+      <c r="P22" s="56"/>
+    </row>
+    <row r="23" spans="1:16" ht="15.75" customHeight="1">
+      <c r="A23" s="55"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="57"/>
+      <c r="D23" s="57"/>
+      <c r="E23" s="57"/>
+      <c r="F23" s="57"/>
+      <c r="G23" s="57"/>
+      <c r="H23" s="57"/>
+      <c r="I23" s="57"/>
+      <c r="J23" s="57"/>
+      <c r="K23" s="57"/>
+      <c r="L23" s="57"/>
+      <c r="M23" s="57"/>
+      <c r="N23" s="57"/>
+      <c r="O23" s="57"/>
+      <c r="P23" s="57"/>
+    </row>
+    <row r="24" spans="1:16" ht="15.75" customHeight="1">
+      <c r="A24" s="58" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="59">
+        <f>SUM(B2:B23)</f>
+        <v>0</v>
+      </c>
+      <c r="C24" s="59">
+        <f t="shared" ref="C24:P24" si="0">SUM(B24-SUM(C2:C23))</f>
+        <v>0</v>
+      </c>
+      <c r="D24" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E24" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F24" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G24" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H24" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I24" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J24" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K24" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L24" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M24" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N24" s="60">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O24" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P24" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="15.75" customHeight="1">
+      <c r="A25" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="59">
+        <f>B24</f>
+        <v>0</v>
+      </c>
+      <c r="C25" s="59">
+        <f t="shared" ref="C25:P25" si="1">B25-$B25/14</f>
+        <v>0</v>
+      </c>
+      <c r="D25" s="59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E25" s="59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F25" s="59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G25" s="59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H25" s="59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I25" s="59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J25" s="59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K25" s="59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L25" s="59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M25" s="59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N25" s="61">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O25" s="59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P25" s="59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" ht="15.75" customHeight="1">
+      <c r="A26" s="62" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="9">
+        <v>0</v>
+      </c>
+      <c r="C26" s="63">
+        <f>B26-C27</f>
+        <v>0</v>
+      </c>
+      <c r="D26" s="63">
+        <f>B26-D27</f>
+        <v>0</v>
+      </c>
+      <c r="E26" s="63">
+        <f>B26-E27</f>
+        <v>0</v>
+      </c>
+      <c r="F26" s="63">
+        <f>B26-F27</f>
+        <v>0</v>
+      </c>
+      <c r="G26" s="63">
+        <f>B26-G27</f>
+        <v>0</v>
+      </c>
+      <c r="H26" s="63">
+        <f>B26-H27</f>
+        <v>0</v>
+      </c>
+      <c r="I26" s="63">
+        <f>B26-I27</f>
+        <v>0</v>
+      </c>
+      <c r="J26" s="63">
+        <f>B26-J27</f>
+        <v>0</v>
+      </c>
+      <c r="K26" s="63">
+        <f>B26-K27</f>
+        <v>0</v>
+      </c>
+      <c r="L26" s="63">
+        <f>B26-L27</f>
+        <v>0</v>
+      </c>
+      <c r="M26" s="63">
+        <f>B26-M27</f>
+        <v>0</v>
+      </c>
+      <c r="N26" s="63">
+        <f>B26-N27</f>
+        <v>0</v>
+      </c>
+      <c r="O26" s="63">
+        <f>B26-O27</f>
+        <v>0</v>
+      </c>
+      <c r="P26" s="63">
+        <f>B26-P27</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" ht="15.75" customHeight="1">
+      <c r="A27" s="62" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" s="9">
+        <v>0</v>
+      </c>
+      <c r="C27" s="9">
+        <v>0</v>
+      </c>
+      <c r="D27" s="9">
+        <v>0</v>
+      </c>
+      <c r="E27" s="9">
+        <v>0</v>
+      </c>
+      <c r="F27" s="9">
+        <v>0</v>
+      </c>
+      <c r="G27" s="9">
+        <v>0</v>
+      </c>
+      <c r="H27" s="9">
+        <v>0</v>
+      </c>
+      <c r="I27" s="9">
+        <v>0</v>
+      </c>
+      <c r="J27" s="9">
+        <v>0</v>
+      </c>
+      <c r="K27" s="9">
+        <v>0</v>
+      </c>
+      <c r="L27" s="9">
+        <v>0</v>
+      </c>
+      <c r="M27" s="9">
+        <v>0</v>
+      </c>
+      <c r="N27" s="9">
+        <v>0</v>
+      </c>
+      <c r="O27" s="9">
+        <v>0</v>
+      </c>
+      <c r="P27" s="9">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2759,11 +3828,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Adding Sprint 5 Chart
</commit_message>
<xml_diff>
--- a/Project Management/BurnDown Charts/BurnDown Chart.xlsx
+++ b/Project Management/BurnDown Charts/BurnDown Chart.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15620" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="1920" yWindow="0" windowWidth="25600" windowHeight="15620" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Table Sprint 5" sheetId="1" r:id="rId1"/>
-    <sheet name="Table Sprint 4" sheetId="2" r:id="rId2"/>
-    <sheet name="Sprint 4 Chart" sheetId="3" r:id="rId3"/>
+    <sheet name="Sprint 5 Chart" sheetId="4" r:id="rId1"/>
+    <sheet name="Table Sprint 5" sheetId="1" r:id="rId2"/>
+    <sheet name="Table Sprint 4" sheetId="2" r:id="rId3"/>
+    <sheet name="Sprint 4 Chart" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="46">
   <si>
     <t>Stories for the Sprint 4</t>
   </si>
@@ -157,6 +158,9 @@
   <si>
     <t>Stories Completed</t>
   </si>
+  <si>
+    <t>Total</t>
+  </si>
 </sst>
 </file>
 
@@ -1189,6 +1193,1250 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
+              <a:t>Sprint</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> 5 BurnDown</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Table Sprint 5'!$A$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Stories Remaining</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Table Sprint 5'!$B$1:$P$1</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Day 1 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Day 2 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Day 3 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Day 4 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Day 5 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Day 6 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Day 7 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Day 8 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Day 9 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Day 10 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Day 11 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Day 12 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Day 13 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Day 14 (Hours)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Table Sprint 5'!$B$26:$P$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Table Sprint 5'!$A$27</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Stories Completed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Table Sprint 5'!$B$1:$P$1</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Day 1 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Day 2 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Day 3 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Day 4 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Day 5 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Day 6 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Day 7 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Day 8 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Day 9 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Day 10 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Day 11 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Day 12 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Day 13 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Day 14 (Hours)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Table Sprint 5'!$B$27:$P$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="-2115866056"/>
+        <c:axId val="-2099120840"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Table Sprint 5'!$A$24</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Remaining Effort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Table Sprint 5'!$B$1:$P$1</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Day 1 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Day 2 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Day 3 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Day 4 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Day 5 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Day 6 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Day 7 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Day 8 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Day 9 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Day 10 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Day 11 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Day 12 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Day 13 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Day 14 (Hours)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Table Sprint 5'!$B$24:$P$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>68.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>68.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>68.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>68.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>68.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>62.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>54.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>49.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>39.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Table Sprint 5'!$A$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ideal Burndown</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Table Sprint 5'!$B$1:$P$1</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Day 1 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Day 2 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Day 3 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Day 4 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Day 5 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Day 6 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Day 7 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Day 8 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Day 9 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Day 10 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Day 11 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Day 12 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Day 13 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Day 14 (Hours)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Table Sprint 5'!$B$25:$P$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>68.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>63.14285714285714</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>58.2857142857143</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>53.42857142857143</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>48.57142857142858</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43.71428571428573</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>38.85714285714288</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>34.00000000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>29.14285714285716</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>24.28571428571431</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>19.42857142857145</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>14.5714285714286</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9.714285714285733</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.857142857142876</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.95399252334028E-14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2115866056"/>
+        <c:axId val="-2099120840"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2115866056"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2099120840"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2099120840"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2115866056"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Sprint</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> 5 BurnDown</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Table Sprint 5'!$A$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Stories Remaining</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Table Sprint 5'!$B$1:$P$1</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Day 1 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Day 2 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Day 3 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Day 4 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Day 5 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Day 6 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Day 7 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Day 8 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Day 9 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Day 10 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Day 11 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Day 12 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Day 13 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Day 14 (Hours)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Table Sprint 5'!$B$26:$P$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Table Sprint 5'!$A$27</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Stories Completed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Table Sprint 5'!$B$1:$P$1</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Day 1 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Day 2 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Day 3 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Day 4 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Day 5 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Day 6 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Day 7 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Day 8 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Day 9 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Day 10 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Day 11 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Day 12 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Day 13 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Day 14 (Hours)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Table Sprint 5'!$B$27:$P$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="-2120718360"/>
+        <c:axId val="-2120715272"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Table Sprint 5'!$A$24</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Remaining Effort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Table Sprint 5'!$B$1:$P$1</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Day 1 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Day 2 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Day 3 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Day 4 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Day 5 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Day 6 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Day 7 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Day 8 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Day 9 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Day 10 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Day 11 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Day 12 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Day 13 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Day 14 (Hours)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Table Sprint 5'!$B$24:$P$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>68.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>68.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>68.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>68.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>68.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>62.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>54.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>49.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>39.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Table Sprint 5'!$A$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ideal Burndown</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Table Sprint 5'!$B$1:$P$1</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Day 1 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Day 2 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Day 3 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Day 4 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Day 5 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Day 6 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Day 7 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Day 8 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Day 9 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Day 10 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Day 11 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Day 12 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Day 13 (Hours)</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Day 14 (Hours)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Table Sprint 5'!$B$25:$P$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>68.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>63.14285714285714</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>58.2857142857143</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>53.42857142857143</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>48.57142857142858</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43.71428571428573</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>38.85714285714288</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>34.00000000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>29.14285714285716</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>24.28571428571431</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>19.42857142857145</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>14.5714285714286</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9.714285714285733</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.857142857142876</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.95399252334028E-14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2120718360"/>
+        <c:axId val="-2120715272"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2120718360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2120715272"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2120715272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2120718360"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
               <a:t>Sprint 4 Burndown</a:t>
             </a:r>
           </a:p>
@@ -1444,8 +2692,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2106116904"/>
-        <c:axId val="-2106009720"/>
+        <c:axId val="-2125869544"/>
+        <c:axId val="-2125866424"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1696,11 +2944,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2106116904"/>
-        <c:axId val="-2106009720"/>
+        <c:axId val="-2125869544"/>
+        <c:axId val="-2125866424"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2106116904"/>
+        <c:axId val="-2125869544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1709,7 +2957,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2106009720"/>
+        <c:crossAx val="-2125866424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1717,7 +2965,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2106009720"/>
+        <c:axId val="-2125866424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1728,7 +2976,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2106116904"/>
+        <c:crossAx val="-2125869544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1751,6 +2999,78 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>736600</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1130300</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2109,10 +3429,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P29" sqref="P29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="J54" sqref="J54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -2125,7 +3465,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>2</v>
@@ -3175,6 +4515,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3183,7 +4524,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P27"/>
   <sheetViews>
@@ -4327,11 +5668,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData/>

</xml_diff>

<commit_message>
Updated with the latest for sprint 5
</commit_message>
<xml_diff>
--- a/Project Management/BurnDown Charts/BurnDown Chart.xlsx
+++ b/Project Management/BurnDown Charts/BurnDown Chart.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="0" windowWidth="25600" windowHeight="15620" tabRatio="500"/>
+    <workbookView xWindow="1100" yWindow="0" windowWidth="25600" windowHeight="15620" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 5 Chart" sheetId="4" r:id="rId1"/>
@@ -166,7 +166,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -208,6 +208,18 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Inconsolata"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="9">
@@ -861,8 +873,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1160,7 +1176,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1326,7 +1346,7 @@
                   <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0.0</c:v>
@@ -1449,10 +1469,10 @@
                   <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4.0</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1468,8 +1488,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2115866056"/>
-        <c:axId val="-2099120840"/>
+        <c:axId val="-2122964120"/>
+        <c:axId val="-2122960872"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1551,46 +1571,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>68.0</c:v>
+                  <c:v>71.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>68.0</c:v>
+                  <c:v>71.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>68.0</c:v>
+                  <c:v>71.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>68.0</c:v>
+                  <c:v>71.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>68.0</c:v>
+                  <c:v>71.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>64.0</c:v>
+                  <c:v>67.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>62.0</c:v>
+                  <c:v>65.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>60.0</c:v>
+                  <c:v>63.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>54.0</c:v>
+                  <c:v>57.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>49.0</c:v>
+                  <c:v>52.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>39.0</c:v>
+                  <c:v>42.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>21.0</c:v>
+                  <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>10.0</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.0</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0.0</c:v>
@@ -1677,49 +1697,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>68.0</c:v>
+                  <c:v>71.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>63.14285714285714</c:v>
+                  <c:v>65.92857142857143</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>58.2857142857143</c:v>
+                  <c:v>60.85714285714286</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>53.42857142857143</c:v>
+                  <c:v>55.7857142857143</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>48.57142857142858</c:v>
+                  <c:v>50.71428571428572</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43.71428571428573</c:v>
+                  <c:v>45.64285714285715</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>38.85714285714288</c:v>
+                  <c:v>40.57142857142858</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>34.00000000000002</c:v>
+                  <c:v>35.50000000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>29.14285714285716</c:v>
+                  <c:v>30.42857142857144</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>24.28571428571431</c:v>
+                  <c:v>25.35714285714288</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>19.42857142857145</c:v>
+                  <c:v>20.28571428571431</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>14.5714285714286</c:v>
+                  <c:v>15.21428571428573</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>9.714285714285733</c:v>
+                  <c:v>10.14285714285716</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4.857142857142876</c:v>
+                  <c:v>5.071428571428592</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.95399252334028E-14</c:v>
+                  <c:v>2.1316282072803E-14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1736,11 +1756,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2115866056"/>
-        <c:axId val="-2099120840"/>
+        <c:axId val="-2122964120"/>
+        <c:axId val="-2122960872"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2115866056"/>
+        <c:axId val="-2122964120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1749,7 +1769,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2099120840"/>
+        <c:crossAx val="-2122960872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1757,7 +1777,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2099120840"/>
+        <c:axId val="-2122960872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1768,7 +1788,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2115866056"/>
+        <c:crossAx val="-2122964120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1815,634 +1835,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Sprint</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> 5 BurnDown</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="stacked"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Table Sprint 5'!$A$26</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Stories Remaining</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Table Sprint 5'!$B$1:$P$1</c:f>
-              <c:strCache>
-                <c:ptCount val="15"/>
-                <c:pt idx="0">
-                  <c:v>Total</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Day 1 (Hours)</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Day 2 (Hours)</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Day 3 (Hours)</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Day 4 (Hours)</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Day 5 (Hours)</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Day 6 (Hours)</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Day 7 (Hours)</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Day 8 (Hours)</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Day 9 (Hours)</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Day 10 (Hours)</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Day 11 (Hours)</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Day 12 (Hours)</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>Day 13 (Hours)</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>Day 14 (Hours)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Table Sprint 5'!$B$26:$P$26</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
-                <c:pt idx="0">
-                  <c:v>11.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>11.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>11.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>11.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>11.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>11.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>11.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>11.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>11.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>11.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>9.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>7.0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Table Sprint 5'!$A$27</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Stories Completed</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Table Sprint 5'!$B$1:$P$1</c:f>
-              <c:strCache>
-                <c:ptCount val="15"/>
-                <c:pt idx="0">
-                  <c:v>Total</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Day 1 (Hours)</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Day 2 (Hours)</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Day 3 (Hours)</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Day 4 (Hours)</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Day 5 (Hours)</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Day 6 (Hours)</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Day 7 (Hours)</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Day 8 (Hours)</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Day 9 (Hours)</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Day 10 (Hours)</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Day 11 (Hours)</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Day 12 (Hours)</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>Day 13 (Hours)</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>Day 14 (Hours)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Table Sprint 5'!$B$27:$P$27</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
-                <c:pt idx="0">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>3.0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:overlap val="100"/>
-        <c:axId val="-2120718360"/>
-        <c:axId val="-2120715272"/>
-      </c:barChart>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Table Sprint 5'!$A$24</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Remaining Effort</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Table Sprint 5'!$B$1:$P$1</c:f>
-              <c:strCache>
-                <c:ptCount val="15"/>
-                <c:pt idx="0">
-                  <c:v>Total</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Day 1 (Hours)</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Day 2 (Hours)</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Day 3 (Hours)</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Day 4 (Hours)</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Day 5 (Hours)</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Day 6 (Hours)</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Day 7 (Hours)</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Day 8 (Hours)</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Day 9 (Hours)</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Day 10 (Hours)</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Day 11 (Hours)</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Day 12 (Hours)</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>Day 13 (Hours)</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>Day 14 (Hours)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Table Sprint 5'!$B$24:$P$24</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
-                <c:pt idx="0">
-                  <c:v>68.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>68.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>68.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>68.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>68.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>64.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>62.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>60.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>54.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>49.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>39.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>21.0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Table Sprint 5'!$A$25</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Ideal Burndown</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Table Sprint 5'!$B$1:$P$1</c:f>
-              <c:strCache>
-                <c:ptCount val="15"/>
-                <c:pt idx="0">
-                  <c:v>Total</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Day 1 (Hours)</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Day 2 (Hours)</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Day 3 (Hours)</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Day 4 (Hours)</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Day 5 (Hours)</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Day 6 (Hours)</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Day 7 (Hours)</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Day 8 (Hours)</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Day 9 (Hours)</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Day 10 (Hours)</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Day 11 (Hours)</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Day 12 (Hours)</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>Day 13 (Hours)</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>Day 14 (Hours)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Table Sprint 5'!$B$25:$P$25</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
-                <c:pt idx="0">
-                  <c:v>68.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>63.14285714285714</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>58.2857142857143</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>53.42857142857143</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>48.57142857142858</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>43.71428571428573</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>38.85714285714288</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>34.00000000000002</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>29.14285714285716</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>24.28571428571431</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>19.42857142857145</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>14.5714285714286</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>9.714285714285733</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>4.857142857142876</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1.95399252334028E-14</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="-2120718360"/>
-        <c:axId val="-2120715272"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="-2120718360"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2120715272"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="-2120715272"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2120718360"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
               <a:t>Sprint 4 Burndown</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2692,8 +2089,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2125869544"/>
-        <c:axId val="-2125866424"/>
+        <c:axId val="2064504040"/>
+        <c:axId val="2064507160"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -2944,11 +2341,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2125869544"/>
-        <c:axId val="-2125866424"/>
+        <c:axId val="2064504040"/>
+        <c:axId val="2064507160"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2125869544"/>
+        <c:axId val="2064504040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2957,7 +2354,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2125866424"/>
+        <c:crossAx val="2064507160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2965,7 +2362,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2125866424"/>
+        <c:axId val="2064507160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2976,14 +2373,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2125869544"/>
+        <c:crossAx val="2064504040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3003,19 +2399,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>368300</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>736600</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -3036,41 +2432,6 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1130300</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>215900</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -3431,8 +2792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P29" sqref="P29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -3451,8 +2812,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="J54" sqref="J54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J52" sqref="J52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -3567,7 +2928,7 @@
       </c>
       <c r="B3" s="10">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C3" s="11">
         <v>0</v>
@@ -3605,11 +2966,11 @@
       <c r="N3" s="11">
         <v>3</v>
       </c>
-      <c r="O3" s="13">
+      <c r="O3" s="99">
         <v>3</v>
       </c>
-      <c r="P3" s="24">
-        <v>0</v>
+      <c r="P3" s="105">
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="12">
@@ -4275,59 +3636,59 @@
       </c>
       <c r="B24" s="101">
         <f>SUM(B2:B23)</f>
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C24" s="101">
         <f t="shared" ref="C24:P24" si="1">SUM(B24-SUM(C2:C23))</f>
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D24" s="101">
         <f t="shared" si="1"/>
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E24" s="101">
         <f t="shared" si="1"/>
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F24" s="101">
         <f t="shared" si="1"/>
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="G24" s="101">
         <f t="shared" si="1"/>
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="H24" s="101">
         <f t="shared" si="1"/>
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="I24" s="101">
         <f t="shared" si="1"/>
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="J24" s="101">
         <f t="shared" si="1"/>
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="K24" s="101">
         <f t="shared" si="1"/>
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="L24" s="101">
         <f t="shared" si="1"/>
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="M24" s="101">
         <f t="shared" si="1"/>
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="N24" s="102">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="O24" s="101">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P24" s="101">
         <f t="shared" si="1"/>
@@ -4340,63 +3701,63 @@
       </c>
       <c r="B25" s="101">
         <f>B24</f>
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C25" s="101">
         <f t="shared" ref="C25:P25" si="2">B25-$B25/14</f>
-        <v>63.142857142857146</v>
+        <v>65.928571428571431</v>
       </c>
       <c r="D25" s="101">
         <f t="shared" si="2"/>
-        <v>58.285714285714292</v>
+        <v>60.857142857142861</v>
       </c>
       <c r="E25" s="101">
         <f t="shared" si="2"/>
-        <v>53.428571428571438</v>
+        <v>55.785714285714292</v>
       </c>
       <c r="F25" s="101">
         <f t="shared" si="2"/>
-        <v>48.571428571428584</v>
+        <v>50.714285714285722</v>
       </c>
       <c r="G25" s="101">
         <f t="shared" si="2"/>
-        <v>43.71428571428573</v>
+        <v>45.642857142857153</v>
       </c>
       <c r="H25" s="101">
         <f t="shared" si="2"/>
-        <v>38.857142857142875</v>
+        <v>40.571428571428584</v>
       </c>
       <c r="I25" s="101">
         <f t="shared" si="2"/>
-        <v>34.000000000000021</v>
+        <v>35.500000000000014</v>
       </c>
       <c r="J25" s="101">
         <f t="shared" si="2"/>
-        <v>29.142857142857164</v>
+        <v>30.428571428571445</v>
       </c>
       <c r="K25" s="101">
         <f t="shared" si="2"/>
-        <v>24.285714285714306</v>
+        <v>25.357142857142875</v>
       </c>
       <c r="L25" s="101">
         <f t="shared" si="2"/>
-        <v>19.428571428571448</v>
+        <v>20.285714285714306</v>
       </c>
       <c r="M25" s="101">
         <f t="shared" si="2"/>
-        <v>14.571428571428591</v>
+        <v>15.214285714285735</v>
       </c>
       <c r="N25" s="103">
         <f t="shared" si="2"/>
-        <v>9.7142857142857331</v>
+        <v>10.142857142857164</v>
       </c>
       <c r="O25" s="101">
         <f t="shared" si="2"/>
-        <v>4.8571428571428763</v>
+        <v>5.0714285714285925</v>
       </c>
       <c r="P25" s="101">
         <f t="shared" si="2"/>
-        <v>1.9539925233402755E-14</v>
+        <v>2.1316282072803006E-14</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="15">
@@ -4456,7 +3817,7 @@
       </c>
       <c r="O26" s="105">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P26" s="105">
         <f t="shared" si="3"/>
@@ -4507,15 +3868,15 @@
         <v>3</v>
       </c>
       <c r="O27" s="13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P27" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>